<commit_message>
EPBDS-8844 Customizing output of a SpreadsheetResult. Tests.
</commit_message>
<xml_diff>
--- a/ITEST/itest.WebService/openl-repository/deployment3/simple3/module1.xlsx
+++ b/ITEST/itest.WebService/openl-repository/deployment3/simple3/module1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\OPENL\ITEST\itest.WebService\openl-repository\deployment3\simple3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79BF4F37-BD69-497D-A9BD-E4EDB460802E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{633BD4AB-D5C5-42E5-A498-5750D22F95D1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6825" yWindow="3390" windowWidth="28845" windowHeight="15225" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15945" yWindow="795" windowWidth="21540" windowHeight="20115" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Rules" sheetId="5" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="125">
   <si>
     <t>Steps</t>
   </si>
@@ -385,6 +385,27 @@
   </si>
   <si>
     <t>= Map m = new HashMap();m.put("key", $Step2);m</t>
+  </si>
+  <si>
+    <t>Step21</t>
+  </si>
+  <si>
+    <t>= spr1(new Double[]{})</t>
+  </si>
+  <si>
+    <t>Step22</t>
+  </si>
+  <si>
+    <t>= (Object[]) $Step21</t>
+  </si>
+  <si>
+    <t>Step23</t>
+  </si>
+  <si>
+    <t>= new Object[]{}</t>
+  </si>
+  <si>
+    <t>= spr(new Double[]{})</t>
   </si>
 </sst>
 </file>
@@ -776,10 +797,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:R65"/>
+  <dimension ref="A2:R64"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -912,7 +933,7 @@
       </c>
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>23</v>
       </c>
@@ -921,7 +942,7 @@
       </c>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B18" s="3" t="s">
         <v>25</v>
       </c>
@@ -929,7 +950,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B19" s="3" t="s">
         <v>28</v>
       </c>
@@ -937,7 +958,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B20" s="3" t="s">
         <v>62</v>
       </c>
@@ -946,7 +967,7 @@
       </c>
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B21" s="3" t="s">
         <v>63</v>
       </c>
@@ -954,7 +975,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B22" s="3" t="s">
         <v>64</v>
       </c>
@@ -962,7 +983,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B23" s="3" t="s">
         <v>65</v>
       </c>
@@ -970,7 +991,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B24" s="3" t="s">
         <v>77</v>
       </c>
@@ -978,15 +999,43 @@
         <v>78</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B25" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="B26" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="B27" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A28" s="1"/>
+      <c r="B28" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="C25">
+      <c r="C28" s="11">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -994,7 +1043,7 @@
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -1002,185 +1051,185 @@
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A31" s="1"/>
-      <c r="B31" s="1"/>
+      <c r="B31" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A32" s="1"/>
       <c r="B32" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
-      <c r="F32" s="1"/>
+        <v>36</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="J32" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K32" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="L32" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="M32" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="N32" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="O32" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="P32" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q32" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="R32" s="1" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A33" s="1"/>
       <c r="B33" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="J33" s="1" t="s">
-        <v>56</v>
+        <v>35</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>60</v>
+        <v>35</v>
       </c>
       <c r="L33" s="1" t="s">
-        <v>61</v>
+        <v>35</v>
       </c>
       <c r="M33" s="1" t="s">
-        <v>71</v>
+        <v>35</v>
       </c>
       <c r="N33" s="1" t="s">
-        <v>72</v>
+        <v>35</v>
       </c>
       <c r="O33" s="1" t="s">
-        <v>73</v>
+        <v>35</v>
       </c>
       <c r="P33" s="1" t="s">
-        <v>74</v>
+        <v>35</v>
       </c>
       <c r="Q33" s="1" t="s">
-        <v>75</v>
+        <v>35</v>
       </c>
       <c r="R33" s="1" t="s">
-        <v>76</v>
+        <v>35</v>
       </c>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A34" s="1"/>
       <c r="B34" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="L34" s="1" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="M34" s="1" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="N34" s="1" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="O34" s="1" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="P34" s="1" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="Q34" s="1" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="R34" s="1" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A35" s="1"/>
-      <c r="B35" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="F35" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="G35" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="H35" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="I35" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="J35" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="K35" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="L35" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="M35" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="N35" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="O35" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="P35" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q35" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="R35" s="1" t="s">
-        <v>40</v>
-      </c>
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+      <c r="F35" s="1"/>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A36" s="1"/>
@@ -1190,185 +1239,177 @@
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A37" s="1"/>
-      <c r="B37" s="1"/>
-      <c r="C37" s="1"/>
-      <c r="D37" s="1"/>
-      <c r="E37" s="1"/>
-      <c r="F37" s="1"/>
+    <row r="43" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="B43" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C43" s="1"/>
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B44" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C44" s="1"/>
+        <v>0</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B45" s="1" t="s">
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>1</v>
+        <v>37</v>
       </c>
     </row>
     <row r="46" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B46" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>37</v>
+      <c r="B46" t="s">
+        <v>2</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B47" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="48" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B48" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="49" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B49" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
     </row>
     <row r="50" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B50" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
     <row r="51" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B51" t="s">
-        <v>14</v>
+      <c r="B51" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
     </row>
     <row r="52" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B52" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="53" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B53" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="54" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B54" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="55" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B55" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
     </row>
     <row r="56" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B56" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
     </row>
     <row r="57" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B57" s="1" t="s">
-        <v>21</v>
+      <c r="B57" t="s">
+        <v>57</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
     </row>
     <row r="58" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B58" t="s">
-        <v>57</v>
+        <v>23</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="59" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B59" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
     </row>
     <row r="60" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B60" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="61" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B61" t="s">
-        <v>28</v>
+        <v>62</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="62" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B62" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="63" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B63" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="64" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B64" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="65" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B65" t="s">
-        <v>65</v>
-      </c>
-      <c r="C65" s="2" t="s">
         <v>79</v>
       </c>
     </row>
@@ -1381,8 +1422,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B2BE8C9-5872-405A-8490-2DC49555BAE6}">
   <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1621,20 +1662,32 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="11"/>
-      <c r="B24" s="11"/>
-      <c r="C24" s="11"/>
+      <c r="B24" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>119</v>
+      </c>
       <c r="D24" s="11"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="11"/>
-      <c r="B25" s="11"/>
-      <c r="C25" s="11"/>
+      <c r="B25" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>121</v>
+      </c>
       <c r="D25" s="11"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="11"/>
-      <c r="B26" s="11"/>
-      <c r="C26" s="11"/>
+      <c r="B26" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>123</v>
+      </c>
       <c r="D26" s="11"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
EPBDS-8844 Byte code generation fails if recursive refereneces between custom spreadsheet results exists. Test is added.
</commit_message>
<xml_diff>
--- a/ITEST/itest.WebService/openl-repository/deployment3/simple3/module1.xlsx
+++ b/ITEST/itest.WebService/openl-repository/deployment3/simple3/module1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\OPENL\ITEST\itest.WebService\openl-repository\deployment3\simple3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1516209-4EC3-4E99-AF6E-74494300F521}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5798FC55-B5C3-4B6D-B151-EE751EF65554}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2925" yWindow="1470" windowWidth="28875" windowHeight="17610" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3308" yWindow="3308" windowWidth="21600" windowHeight="11535" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Rules" sheetId="5" r:id="rId1"/>
@@ -19,11 +19,12 @@
     <sheet name="mysprs" sheetId="8" r:id="rId4"/>
     <sheet name="mysprs2" sheetId="9" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="127">
   <si>
     <t>Steps</t>
   </si>
@@ -409,6 +410,9 @@
   </si>
   <si>
     <t>detailedPlainModel</t>
+  </si>
+  <si>
+    <t>= false ? spr(1) : null</t>
   </si>
 </sst>
 </file>
@@ -802,28 +806,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:R65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="33.28515625" customWidth="1"/>
+    <col min="3" max="3" width="33.265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
         <v>6</v>
@@ -831,7 +835,7 @@
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B5" s="11" t="s">
         <v>85</v>
       </c>
@@ -842,7 +846,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="1"/>
       <c r="B6" s="1" t="s">
         <v>0</v>
@@ -852,7 +856,7 @@
       </c>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
         <v>2</v>
@@ -862,7 +866,7 @@
       </c>
       <c r="D7" s="1"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="1"/>
       <c r="B8" s="3" t="s">
         <v>3</v>
@@ -872,7 +876,7 @@
       </c>
       <c r="D8" s="1"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="1"/>
       <c r="B9" s="1" t="s">
         <v>10</v>
@@ -882,7 +886,7 @@
       </c>
       <c r="D9" s="1"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B10" s="3" t="s">
         <v>13</v>
       </c>
@@ -890,7 +894,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B11" s="1" t="s">
         <v>14</v>
       </c>
@@ -898,7 +902,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B12" s="3" t="s">
         <v>15</v>
       </c>
@@ -906,7 +910,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B13" s="1" t="s">
         <v>16</v>
       </c>
@@ -914,7 +918,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B14" s="3" t="s">
         <v>18</v>
       </c>
@@ -922,7 +926,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B15" s="1" t="s">
         <v>19</v>
       </c>
@@ -930,7 +934,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B16" s="3" t="s">
         <v>20</v>
       </c>
@@ -938,7 +942,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B17" s="3" t="s">
         <v>21</v>
       </c>
@@ -947,7 +951,7 @@
       </c>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B18" t="s">
         <v>23</v>
       </c>
@@ -956,7 +960,7 @@
       </c>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B19" s="3" t="s">
         <v>25</v>
       </c>
@@ -964,7 +968,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B20" s="3" t="s">
         <v>28</v>
       </c>
@@ -972,7 +976,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B21" s="3" t="s">
         <v>62</v>
       </c>
@@ -981,7 +985,7 @@
       </c>
       <c r="D21" s="1"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B22" s="3" t="s">
         <v>63</v>
       </c>
@@ -989,7 +993,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B23" s="3" t="s">
         <v>64</v>
       </c>
@@ -997,7 +1001,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B24" s="3" t="s">
         <v>65</v>
       </c>
@@ -1005,7 +1009,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B25" s="3" t="s">
         <v>77</v>
       </c>
@@ -1013,7 +1017,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B26" s="3" t="s">
         <v>118</v>
       </c>
@@ -1021,7 +1025,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B27" s="3" t="s">
         <v>120</v>
       </c>
@@ -1029,7 +1033,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B28" s="3" t="s">
         <v>122</v>
       </c>
@@ -1037,7 +1041,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" s="1"/>
       <c r="B29" s="3" t="s">
         <v>110</v>
@@ -1049,7 +1053,7 @@
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -1057,7 +1061,7 @@
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -1065,7 +1069,7 @@
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32" s="1"/>
       <c r="B32" s="1" t="s">
         <v>34</v>
@@ -1075,7 +1079,7 @@
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A33" s="1"/>
       <c r="B33" s="1" t="s">
         <v>36</v>
@@ -1129,7 +1133,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A34" s="1"/>
       <c r="B34" s="1" t="s">
         <v>35</v>
@@ -1183,7 +1187,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A35" s="1"/>
       <c r="B35" s="1" t="s">
         <v>37</v>
@@ -1237,7 +1241,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -1245,7 +1249,7 @@
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -1253,13 +1257,13 @@
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B44" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C44" s="1"/>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B45" s="1" t="s">
         <v>0</v>
       </c>
@@ -1267,7 +1271,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B46" s="1" t="s">
         <v>38</v>
       </c>
@@ -1275,7 +1279,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B47" t="s">
         <v>2</v>
       </c>
@@ -1283,7 +1287,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B48" t="s">
         <v>3</v>
       </c>
@@ -1291,7 +1295,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B49" t="s">
         <v>10</v>
       </c>
@@ -1299,7 +1303,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B50" t="s">
         <v>13</v>
       </c>
@@ -1307,7 +1311,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="51" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B51" t="s">
         <v>14</v>
       </c>
@@ -1315,7 +1319,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="52" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B52" s="1" t="s">
         <v>15</v>
       </c>
@@ -1323,7 +1327,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="53" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B53" s="1" t="s">
         <v>16</v>
       </c>
@@ -1331,7 +1335,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="54" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B54" s="1" t="s">
         <v>18</v>
       </c>
@@ -1339,7 +1343,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="55" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B55" s="1" t="s">
         <v>19</v>
       </c>
@@ -1347,7 +1351,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B56" s="1" t="s">
         <v>20</v>
       </c>
@@ -1355,7 +1359,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="57" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B57" s="1" t="s">
         <v>21</v>
       </c>
@@ -1363,7 +1367,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="58" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B58" t="s">
         <v>57</v>
       </c>
@@ -1371,7 +1375,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="59" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B59" t="s">
         <v>23</v>
       </c>
@@ -1379,7 +1383,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="60" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B60" t="s">
         <v>25</v>
       </c>
@@ -1387,7 +1391,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="61" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="61" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B61" t="s">
         <v>28</v>
       </c>
@@ -1395,7 +1399,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="62" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="62" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B62" t="s">
         <v>62</v>
       </c>
@@ -1403,7 +1407,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="63" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="63" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B63" t="s">
         <v>63</v>
       </c>
@@ -1411,7 +1415,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="64" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="64" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B64" t="s">
         <v>64</v>
       </c>
@@ -1419,7 +1423,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="65" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="65" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B65" t="s">
         <v>65</v>
       </c>
@@ -1440,9 +1444,9 @@
       <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -1450,7 +1454,7 @@
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1458,7 +1462,7 @@
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
         <v>9</v>
@@ -1468,7 +1472,7 @@
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
         <v>0</v>
@@ -1480,7 +1484,7 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
         <v>2</v>
@@ -1492,7 +1496,7 @@
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="1"/>
       <c r="B6" s="1" t="s">
         <v>3</v>
@@ -1504,7 +1508,7 @@
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
         <v>10</v>
@@ -1516,7 +1520,7 @@
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="1"/>
       <c r="B8" s="1" t="s">
         <v>13</v>
@@ -1528,7 +1532,7 @@
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="1"/>
       <c r="B9" s="1" t="s">
         <v>14</v>
@@ -1540,7 +1544,7 @@
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="1"/>
       <c r="B10" s="1" t="s">
         <v>15</v>
@@ -1552,7 +1556,7 @@
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B11" s="1" t="s">
         <v>16</v>
       </c>
@@ -1560,7 +1564,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B12" s="1" t="s">
         <v>18</v>
       </c>
@@ -1568,7 +1572,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B13" s="1" t="s">
         <v>19</v>
       </c>
@@ -1576,7 +1580,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B14" s="1" t="s">
         <v>20</v>
       </c>
@@ -1584,7 +1588,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" s="11"/>
       <c r="B15" s="11" t="s">
         <v>21</v>
@@ -1594,7 +1598,7 @@
       </c>
       <c r="D15" s="11"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" s="11"/>
       <c r="B16" s="11" t="s">
         <v>23</v>
@@ -1604,7 +1608,7 @@
       </c>
       <c r="D16" s="11"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" s="11"/>
       <c r="B17" s="11" t="s">
         <v>25</v>
@@ -1614,7 +1618,7 @@
       </c>
       <c r="D17" s="11"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" s="11"/>
       <c r="B18" s="11" t="s">
         <v>28</v>
@@ -1624,7 +1628,7 @@
       </c>
       <c r="D18" s="11"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" s="11"/>
       <c r="B19" s="11" t="s">
         <v>62</v>
@@ -1634,7 +1638,7 @@
       </c>
       <c r="D19" s="11"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" s="11"/>
       <c r="B20" s="11" t="s">
         <v>63</v>
@@ -1644,7 +1648,7 @@
       </c>
       <c r="D20" s="11"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" s="11"/>
       <c r="B21" s="11" t="s">
         <v>64</v>
@@ -1654,7 +1658,7 @@
       </c>
       <c r="D21" s="11"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" s="11"/>
       <c r="B22" s="11" t="s">
         <v>65</v>
@@ -1664,7 +1668,7 @@
       </c>
       <c r="D22" s="11"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" s="11"/>
       <c r="B23" s="11" t="s">
         <v>77</v>
@@ -1674,7 +1678,7 @@
       </c>
       <c r="D23" s="11"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" s="11"/>
       <c r="B24" s="11" t="s">
         <v>118</v>
@@ -1684,7 +1688,7 @@
       </c>
       <c r="D24" s="11"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" s="11"/>
       <c r="B25" s="11" t="s">
         <v>120</v>
@@ -1694,7 +1698,7 @@
       </c>
       <c r="D25" s="11"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" s="11"/>
       <c r="B26" s="11" t="s">
         <v>122</v>
@@ -1704,13 +1708,13 @@
       </c>
       <c r="D26" s="11"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" s="11"/>
       <c r="B27" s="11"/>
       <c r="C27" s="11"/>
       <c r="D27" s="11"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" s="11"/>
       <c r="B28" s="11"/>
       <c r="C28" s="11"/>
@@ -1725,19 +1729,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0594453C-8787-494B-B55E-35A8780F32ED}">
   <dimension ref="B3:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B3" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="1"/>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
@@ -1745,7 +1749,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B5" s="1" t="s">
         <v>2</v>
       </c>
@@ -1753,9 +1757,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B6" s="1"/>
-      <c r="C6" s="2"/>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>126</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1770,15 +1778,15 @@
       <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="2" spans="2:4" s="11" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="3" spans="2:4" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:4" s="11" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="2:4" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B3" s="11" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="4" spans="2:4" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:4" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B4" s="11" t="s">
         <v>0</v>
       </c>
@@ -1786,7 +1794,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B5" s="11" t="s">
         <v>2</v>
       </c>
@@ -1794,35 +1802,35 @@
         <v>91</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B9" s="12"/>
       <c r="D9" s="13"/>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B13" s="11"/>
       <c r="C13" s="10"/>
       <c r="D13" s="9"/>
     </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B16" s="1" t="s">
         <v>80</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B17" s="7" t="s">
         <v>85</v>
       </c>
@@ -1833,7 +1841,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B18" s="1" t="s">
         <v>0</v>
       </c>
@@ -1844,7 +1852,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B19" s="1" t="s">
         <v>84</v>
       </c>
@@ -1855,7 +1863,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B20" s="1" t="s">
         <v>82</v>
       </c>
@@ -1866,18 +1874,18 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B21" s="6"/>
       <c r="C21" s="5"/>
       <c r="D21" s="4"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="11"/>
       <c r="B22" s="11"/>
       <c r="C22" s="11"/>
       <c r="D22" s="11"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="11"/>
       <c r="B23" s="11" t="s">
         <v>93</v>
@@ -1885,7 +1893,7 @@
       <c r="C23" s="11"/>
       <c r="D23" s="11"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="11"/>
       <c r="B24" s="11" t="s">
         <v>90</v>
@@ -1898,7 +1906,7 @@
       </c>
       <c r="E24" s="11"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="11"/>
       <c r="B25" s="11" t="s">
         <v>89</v>
@@ -1911,7 +1919,7 @@
       </c>
       <c r="E25" s="11"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" s="11"/>
       <c r="B26" s="11" t="s">
         <v>87</v>
@@ -1923,7 +1931,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" s="11"/>
       <c r="B27" s="11" t="s">
         <v>88</v>
@@ -1946,16 +1954,16 @@
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B3" s="11" t="s">
         <v>97</v>
       </c>
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B4" s="11" t="s">
         <v>0</v>
       </c>
@@ -1964,7 +1972,7 @@
       </c>
       <c r="D4" s="11"/>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B5" s="11" t="s">
         <v>2</v>
       </c>
@@ -1973,64 +1981,64 @@
       </c>
       <c r="D5" s="11"/>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
       <c r="D6" s="11"/>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B7" s="11"/>
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B9" s="13"/>
       <c r="C9" s="11"/>
       <c r="D9" s="13"/>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B10" s="11"/>
       <c r="C10" s="11"/>
       <c r="D10" s="11"/>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B11" s="11"/>
       <c r="C11" s="11"/>
       <c r="D11" s="11"/>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B12" s="11"/>
       <c r="C12" s="11"/>
       <c r="D12" s="11"/>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B13" s="11"/>
       <c r="C13" s="11"/>
       <c r="D13" s="11"/>
     </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B14" s="11"/>
       <c r="C14" s="11"/>
       <c r="D14" s="11"/>
     </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B15" s="11"/>
       <c r="C15" s="11"/>
       <c r="D15" s="11"/>
     </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B16" s="11" t="s">
         <v>103</v>
       </c>
       <c r="C16" s="11"/>
       <c r="D16" s="11"/>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B17" s="13" t="s">
         <v>85</v>
       </c>
@@ -2041,7 +2049,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B18" s="11" t="s">
         <v>0</v>
       </c>
@@ -2052,7 +2060,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B19" s="11" t="s">
         <v>99</v>
       </c>
@@ -2063,7 +2071,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B20" s="11" t="s">
         <v>100</v>
       </c>
@@ -2074,24 +2082,24 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B21" s="11"/>
       <c r="C21" s="11"/>
       <c r="D21" s="11"/>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B22" s="11"/>
       <c r="C22" s="11"/>
       <c r="D22" s="11"/>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B23" s="11" t="s">
         <v>104</v>
       </c>
       <c r="C23" s="11"/>
       <c r="D23" s="11"/>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B24" s="11" t="s">
         <v>90</v>
       </c>
@@ -2108,7 +2116,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B25" s="11" t="s">
         <v>89</v>
       </c>
@@ -2119,7 +2127,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B26" s="11" t="s">
         <v>87</v>
       </c>
@@ -2132,7 +2140,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B27" s="11" t="s">
         <v>88</v>
       </c>

</xml_diff>

<commit_message>
EPBDS-8844 Support convertation to SPR Beans if method return array of custom spreadsheet results
</commit_message>
<xml_diff>
--- a/ITEST/itest.WebService/openl-repository/deployment3/simple3/module1.xlsx
+++ b/ITEST/itest.WebService/openl-repository/deployment3/simple3/module1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\OPENL\ITEST\itest.WebService\openl-repository\deployment3\simple3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5798FC55-B5C3-4B6D-B151-EE751EF65554}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F36C708A-F2ED-43DC-A4BE-02579CD9C3CB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3308" yWindow="3308" windowWidth="21600" windowHeight="11535" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15945" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Rules" sheetId="5" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="131">
   <si>
     <t>Steps</t>
   </si>
@@ -413,6 +413,18 @@
   </si>
   <si>
     <t>= false ? spr(1) : null</t>
+  </si>
+  <si>
+    <t>RETURN</t>
+  </si>
+  <si>
+    <t>= spr1(new Double[]{1,2})</t>
+  </si>
+  <si>
+    <t>Spreadsheet SpreadsheetResult[] arrSpreadsheetResult()</t>
+  </si>
+  <si>
+    <t>Spreadsheet SpreadsheetResultspr1[] arrSpreadsheetResultspr1()</t>
   </si>
 </sst>
 </file>
@@ -1727,21 +1739,21 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0594453C-8787-494B-B55E-35A8780F32ED}">
-  <dimension ref="B3:C6"/>
+  <dimension ref="B3:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B3" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="1"/>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
@@ -1749,7 +1761,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B5" s="1" t="s">
         <v>2</v>
       </c>
@@ -1757,13 +1769,72 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>126</v>
       </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B11" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B12" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B13" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B14" s="11"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B17" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B18" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D18" s="11"/>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B19" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="D19" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
EPBDS-9550 Repacking result array if types aren't valid
</commit_message>
<xml_diff>
--- a/ITEST/itest.WebService/openl-repository/deployment3/simple3/module1.xlsx
+++ b/ITEST/itest.WebService/openl-repository/deployment3/simple3/module1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\OPENL\ITEST\itest.WebService\openl-repository\deployment3\simple3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\ITEST\itest.WebService\openl-repository\deployment3\simple3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F36C708A-F2ED-43DC-A4BE-02579CD9C3CB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DD1E007-2276-4045-A760-CF4FA0E8FBF4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15945" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="6165" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Rules" sheetId="5" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="132">
   <si>
     <t>Steps</t>
   </si>
@@ -425,6 +425,9 @@
   </si>
   <si>
     <t>Spreadsheet SpreadsheetResultspr1[] arrSpreadsheetResultspr1()</t>
+  </si>
+  <si>
+    <t>Spreadsheet Object[] arrObjSpreadsheetResult()</t>
   </si>
 </sst>
 </file>
@@ -822,24 +825,24 @@
       <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="3" max="3" width="33.265625" customWidth="1"/>
+    <col min="3" max="3" width="33.27734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
         <v>6</v>
@@ -847,7 +850,7 @@
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B5" s="11" t="s">
         <v>85</v>
       </c>
@@ -858,7 +861,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A6" s="1"/>
       <c r="B6" s="1" t="s">
         <v>0</v>
@@ -868,7 +871,7 @@
       </c>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
         <v>2</v>
@@ -878,7 +881,7 @@
       </c>
       <c r="D7" s="1"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A8" s="1"/>
       <c r="B8" s="3" t="s">
         <v>3</v>
@@ -888,7 +891,7 @@
       </c>
       <c r="D8" s="1"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A9" s="1"/>
       <c r="B9" s="1" t="s">
         <v>10</v>
@@ -898,7 +901,7 @@
       </c>
       <c r="D9" s="1"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.4">
       <c r="B10" s="3" t="s">
         <v>13</v>
       </c>
@@ -906,7 +909,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.4">
       <c r="B11" s="1" t="s">
         <v>14</v>
       </c>
@@ -914,7 +917,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.4">
       <c r="B12" s="3" t="s">
         <v>15</v>
       </c>
@@ -922,7 +925,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.4">
       <c r="B13" s="1" t="s">
         <v>16</v>
       </c>
@@ -930,7 +933,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.4">
       <c r="B14" s="3" t="s">
         <v>18</v>
       </c>
@@ -938,7 +941,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.4">
       <c r="B15" s="1" t="s">
         <v>19</v>
       </c>
@@ -946,7 +949,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.4">
       <c r="B16" s="3" t="s">
         <v>20</v>
       </c>
@@ -954,7 +957,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B17" s="3" t="s">
         <v>21</v>
       </c>
@@ -963,7 +966,7 @@
       </c>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B18" t="s">
         <v>23</v>
       </c>
@@ -972,7 +975,7 @@
       </c>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B19" s="3" t="s">
         <v>25</v>
       </c>
@@ -980,7 +983,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B20" s="3" t="s">
         <v>28</v>
       </c>
@@ -988,7 +991,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B21" s="3" t="s">
         <v>62</v>
       </c>
@@ -997,7 +1000,7 @@
       </c>
       <c r="D21" s="1"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B22" s="3" t="s">
         <v>63</v>
       </c>
@@ -1005,7 +1008,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B23" s="3" t="s">
         <v>64</v>
       </c>
@@ -1013,7 +1016,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B24" s="3" t="s">
         <v>65</v>
       </c>
@@ -1021,7 +1024,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B25" s="3" t="s">
         <v>77</v>
       </c>
@@ -1029,7 +1032,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B26" s="3" t="s">
         <v>118</v>
       </c>
@@ -1037,7 +1040,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B27" s="3" t="s">
         <v>120</v>
       </c>
@@ -1045,7 +1048,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B28" s="3" t="s">
         <v>122</v>
       </c>
@@ -1053,7 +1056,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A29" s="1"/>
       <c r="B29" s="3" t="s">
         <v>110</v>
@@ -1065,7 +1068,7 @@
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -1073,7 +1076,7 @@
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -1081,7 +1084,7 @@
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A32" s="1"/>
       <c r="B32" s="1" t="s">
         <v>34</v>
@@ -1091,7 +1094,7 @@
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A33" s="1"/>
       <c r="B33" s="1" t="s">
         <v>36</v>
@@ -1145,7 +1148,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A34" s="1"/>
       <c r="B34" s="1" t="s">
         <v>35</v>
@@ -1199,7 +1202,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A35" s="1"/>
       <c r="B35" s="1" t="s">
         <v>37</v>
@@ -1253,7 +1256,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -1261,7 +1264,7 @@
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -1269,13 +1272,13 @@
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.4">
       <c r="B44" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C44" s="1"/>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.4">
       <c r="B45" s="1" t="s">
         <v>0</v>
       </c>
@@ -1283,7 +1286,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.4">
       <c r="B46" s="1" t="s">
         <v>38</v>
       </c>
@@ -1291,7 +1294,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.4">
       <c r="B47" t="s">
         <v>2</v>
       </c>
@@ -1299,7 +1302,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.4">
       <c r="B48" t="s">
         <v>3</v>
       </c>
@@ -1307,7 +1310,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="49" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B49" t="s">
         <v>10</v>
       </c>
@@ -1315,7 +1318,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="50" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B50" t="s">
         <v>13</v>
       </c>
@@ -1323,7 +1326,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="51" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="51" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B51" t="s">
         <v>14</v>
       </c>
@@ -1331,7 +1334,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="52" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="52" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B52" s="1" t="s">
         <v>15</v>
       </c>
@@ -1339,7 +1342,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="53" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="53" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B53" s="1" t="s">
         <v>16</v>
       </c>
@@ -1347,7 +1350,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="54" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="54" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B54" s="1" t="s">
         <v>18</v>
       </c>
@@ -1355,7 +1358,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="55" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="55" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B55" s="1" t="s">
         <v>19</v>
       </c>
@@ -1363,7 +1366,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="56" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B56" s="1" t="s">
         <v>20</v>
       </c>
@@ -1371,7 +1374,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="57" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="57" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B57" s="1" t="s">
         <v>21</v>
       </c>
@@ -1379,7 +1382,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="58" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="58" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B58" t="s">
         <v>57</v>
       </c>
@@ -1387,7 +1390,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="59" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="59" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B59" t="s">
         <v>23</v>
       </c>
@@ -1395,7 +1398,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="60" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="60" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B60" t="s">
         <v>25</v>
       </c>
@@ -1403,7 +1406,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="61" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="61" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B61" t="s">
         <v>28</v>
       </c>
@@ -1411,7 +1414,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="62" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="62" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B62" t="s">
         <v>62</v>
       </c>
@@ -1419,7 +1422,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="63" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="63" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B63" t="s">
         <v>63</v>
       </c>
@@ -1427,7 +1430,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="64" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="64" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B64" t="s">
         <v>64</v>
       </c>
@@ -1435,7 +1438,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="65" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="65" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B65" t="s">
         <v>65</v>
       </c>
@@ -1456,9 +1459,9 @@
       <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -1466,7 +1469,7 @@
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1474,7 +1477,7 @@
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
         <v>9</v>
@@ -1484,7 +1487,7 @@
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
         <v>0</v>
@@ -1496,7 +1499,7 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
         <v>2</v>
@@ -1508,7 +1511,7 @@
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A6" s="1"/>
       <c r="B6" s="1" t="s">
         <v>3</v>
@@ -1520,7 +1523,7 @@
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
         <v>10</v>
@@ -1532,7 +1535,7 @@
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A8" s="1"/>
       <c r="B8" s="1" t="s">
         <v>13</v>
@@ -1544,7 +1547,7 @@
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A9" s="1"/>
       <c r="B9" s="1" t="s">
         <v>14</v>
@@ -1556,7 +1559,7 @@
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A10" s="1"/>
       <c r="B10" s="1" t="s">
         <v>15</v>
@@ -1568,7 +1571,7 @@
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B11" s="1" t="s">
         <v>16</v>
       </c>
@@ -1576,7 +1579,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B12" s="1" t="s">
         <v>18</v>
       </c>
@@ -1584,7 +1587,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B13" s="1" t="s">
         <v>19</v>
       </c>
@@ -1592,7 +1595,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B14" s="1" t="s">
         <v>20</v>
       </c>
@@ -1600,7 +1603,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A15" s="11"/>
       <c r="B15" s="11" t="s">
         <v>21</v>
@@ -1610,7 +1613,7 @@
       </c>
       <c r="D15" s="11"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A16" s="11"/>
       <c r="B16" s="11" t="s">
         <v>23</v>
@@ -1620,7 +1623,7 @@
       </c>
       <c r="D16" s="11"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A17" s="11"/>
       <c r="B17" s="11" t="s">
         <v>25</v>
@@ -1630,7 +1633,7 @@
       </c>
       <c r="D17" s="11"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A18" s="11"/>
       <c r="B18" s="11" t="s">
         <v>28</v>
@@ -1640,7 +1643,7 @@
       </c>
       <c r="D18" s="11"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A19" s="11"/>
       <c r="B19" s="11" t="s">
         <v>62</v>
@@ -1650,7 +1653,7 @@
       </c>
       <c r="D19" s="11"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A20" s="11"/>
       <c r="B20" s="11" t="s">
         <v>63</v>
@@ -1660,7 +1663,7 @@
       </c>
       <c r="D20" s="11"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A21" s="11"/>
       <c r="B21" s="11" t="s">
         <v>64</v>
@@ -1670,7 +1673,7 @@
       </c>
       <c r="D21" s="11"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A22" s="11"/>
       <c r="B22" s="11" t="s">
         <v>65</v>
@@ -1680,7 +1683,7 @@
       </c>
       <c r="D22" s="11"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A23" s="11"/>
       <c r="B23" s="11" t="s">
         <v>77</v>
@@ -1690,7 +1693,7 @@
       </c>
       <c r="D23" s="11"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A24" s="11"/>
       <c r="B24" s="11" t="s">
         <v>118</v>
@@ -1700,7 +1703,7 @@
       </c>
       <c r="D24" s="11"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A25" s="11"/>
       <c r="B25" s="11" t="s">
         <v>120</v>
@@ -1710,7 +1713,7 @@
       </c>
       <c r="D25" s="11"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A26" s="11"/>
       <c r="B26" s="11" t="s">
         <v>122</v>
@@ -1720,13 +1723,13 @@
       </c>
       <c r="D26" s="11"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A27" s="11"/>
       <c r="B27" s="11"/>
       <c r="C27" s="11"/>
       <c r="D27" s="11"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A28" s="11"/>
       <c r="B28" s="11"/>
       <c r="C28" s="11"/>
@@ -1739,21 +1742,21 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0594453C-8787-494B-B55E-35A8780F32ED}">
-  <dimension ref="B3:E19"/>
+  <dimension ref="B3:E23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B3" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="1"/>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
@@ -1761,7 +1764,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B5" s="1" t="s">
         <v>2</v>
       </c>
@@ -1769,7 +1772,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
@@ -1777,7 +1780,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B11" s="11" t="s">
         <v>129</v>
       </c>
@@ -1785,7 +1788,7 @@
       <c r="D11" s="11"/>
       <c r="E11" s="11"/>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B12" s="11" t="s">
         <v>0</v>
       </c>
@@ -1795,7 +1798,7 @@
       <c r="D12" s="11"/>
       <c r="E12" s="11"/>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B13" s="11" t="s">
         <v>127</v>
       </c>
@@ -1805,20 +1808,20 @@
       <c r="D13" s="11"/>
       <c r="E13" s="11"/>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B14" s="11"/>
       <c r="C14" s="2"/>
       <c r="D14" s="11"/>
       <c r="E14" s="11"/>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B17" s="11" t="s">
         <v>130</v>
       </c>
       <c r="C17" s="11"/>
       <c r="D17" s="11"/>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B18" s="11" t="s">
         <v>0</v>
       </c>
@@ -1827,7 +1830,7 @@
       </c>
       <c r="D18" s="11"/>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B19" s="11" t="s">
         <v>127</v>
       </c>
@@ -1835,6 +1838,34 @@
         <v>128</v>
       </c>
       <c r="D19" s="11"/>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="B21" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="C21" s="11"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="11"/>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="B22" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D22" s="11"/>
+      <c r="E22" s="11"/>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="B23" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="D23" s="11"/>
+      <c r="E23" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1849,15 +1880,15 @@
       <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="2" spans="2:4" s="11" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="2:4" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:4" s="11" customFormat="1" x14ac:dyDescent="0.4"/>
+    <row r="3" spans="2:4" s="11" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B3" s="11" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="4" spans="2:4" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:4" s="11" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B4" s="11" t="s">
         <v>0</v>
       </c>
@@ -1865,7 +1896,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B5" s="11" t="s">
         <v>2</v>
       </c>
@@ -1873,35 +1904,35 @@
         <v>91</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B9" s="12"/>
       <c r="D9" s="13"/>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B13" s="11"/>
       <c r="C13" s="10"/>
       <c r="D13" s="9"/>
     </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B16" s="1" t="s">
         <v>80</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B17" s="7" t="s">
         <v>85</v>
       </c>
@@ -1912,7 +1943,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B18" s="1" t="s">
         <v>0</v>
       </c>
@@ -1923,7 +1954,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B19" s="1" t="s">
         <v>84</v>
       </c>
@@ -1934,7 +1965,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B20" s="1" t="s">
         <v>82</v>
       </c>
@@ -1945,18 +1976,18 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B21" s="6"/>
       <c r="C21" s="5"/>
       <c r="D21" s="4"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A22" s="11"/>
       <c r="B22" s="11"/>
       <c r="C22" s="11"/>
       <c r="D22" s="11"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A23" s="11"/>
       <c r="B23" s="11" t="s">
         <v>93</v>
@@ -1964,7 +1995,7 @@
       <c r="C23" s="11"/>
       <c r="D23" s="11"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A24" s="11"/>
       <c r="B24" s="11" t="s">
         <v>90</v>
@@ -1977,7 +2008,7 @@
       </c>
       <c r="E24" s="11"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A25" s="11"/>
       <c r="B25" s="11" t="s">
         <v>89</v>
@@ -1990,7 +2021,7 @@
       </c>
       <c r="E25" s="11"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A26" s="11"/>
       <c r="B26" s="11" t="s">
         <v>87</v>
@@ -2002,7 +2033,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A27" s="11"/>
       <c r="B27" s="11" t="s">
         <v>88</v>
@@ -2025,16 +2056,16 @@
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B3" s="11" t="s">
         <v>97</v>
       </c>
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B4" s="11" t="s">
         <v>0</v>
       </c>
@@ -2043,7 +2074,7 @@
       </c>
       <c r="D4" s="11"/>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B5" s="11" t="s">
         <v>2</v>
       </c>
@@ -2052,64 +2083,64 @@
       </c>
       <c r="D5" s="11"/>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
       <c r="D6" s="11"/>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B7" s="11"/>
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B9" s="13"/>
       <c r="C9" s="11"/>
       <c r="D9" s="13"/>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B10" s="11"/>
       <c r="C10" s="11"/>
       <c r="D10" s="11"/>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B11" s="11"/>
       <c r="C11" s="11"/>
       <c r="D11" s="11"/>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B12" s="11"/>
       <c r="C12" s="11"/>
       <c r="D12" s="11"/>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B13" s="11"/>
       <c r="C13" s="11"/>
       <c r="D13" s="11"/>
     </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B14" s="11"/>
       <c r="C14" s="11"/>
       <c r="D14" s="11"/>
     </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B15" s="11"/>
       <c r="C15" s="11"/>
       <c r="D15" s="11"/>
     </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B16" s="11" t="s">
         <v>103</v>
       </c>
       <c r="C16" s="11"/>
       <c r="D16" s="11"/>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B17" s="13" t="s">
         <v>85</v>
       </c>
@@ -2120,7 +2151,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B18" s="11" t="s">
         <v>0</v>
       </c>
@@ -2131,7 +2162,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B19" s="11" t="s">
         <v>99</v>
       </c>
@@ -2142,7 +2173,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B20" s="11" t="s">
         <v>100</v>
       </c>
@@ -2153,24 +2184,24 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B21" s="11"/>
       <c r="C21" s="11"/>
       <c r="D21" s="11"/>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B22" s="11"/>
       <c r="C22" s="11"/>
       <c r="D22" s="11"/>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B23" s="11" t="s">
         <v>104</v>
       </c>
       <c r="C23" s="11"/>
       <c r="D23" s="11"/>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B24" s="11" t="s">
         <v>90</v>
       </c>
@@ -2187,7 +2218,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B25" s="11" t="s">
         <v>89</v>
       </c>
@@ -2198,7 +2229,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B26" s="11" t="s">
         <v>87</v>
       </c>
@@ -2211,7 +2242,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B27" s="11" t="s">
         <v>88</v>
       </c>

</xml_diff>

<commit_message>
EPBDS-9540 Hide internal methods. Fix collision resolving
</commit_message>
<xml_diff>
--- a/ITEST/itest.WebService/openl-repository/deployment3/simple3/module1.xlsx
+++ b/ITEST/itest.WebService/openl-repository/deployment3/simple3/module1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\ITEST\itest.WebService\openl-repository\deployment3\simple3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OpenL\ITEST\itest.WebService\openl-repository\deployment3\simple3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DD1E007-2276-4045-A760-CF4FA0E8FBF4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F47EA61C-5B25-4715-ACE5-C380ABE7FEB3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="6165" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Rules" sheetId="5" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="131">
   <si>
     <t>Steps</t>
   </si>
@@ -128,9 +128,6 @@
   </si>
   <si>
     <t>=main()</t>
-  </si>
-  <si>
-    <t>= $Step1.toPlain()</t>
   </si>
   <si>
     <t>= $Step1.toMap()</t>
@@ -483,7 +480,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -499,9 +496,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -539,7 +536,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -645,7 +642,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -819,30 +816,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:R65"/>
+  <dimension ref="A2:R64"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A49" sqref="A49:XFD49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="33.27734375" customWidth="1"/>
+    <col min="3" max="3" width="33.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
         <v>6</v>
@@ -850,18 +847,18 @@
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B5" s="11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
       <c r="B6" s="1" t="s">
         <v>0</v>
@@ -871,7 +868,7 @@
       </c>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
         <v>2</v>
@@ -881,7 +878,7 @@
       </c>
       <c r="D7" s="1"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
       <c r="B8" s="3" t="s">
         <v>3</v>
@@ -891,7 +888,7 @@
       </c>
       <c r="D8" s="1"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>
       <c r="B9" s="1" t="s">
         <v>10</v>
@@ -901,7 +898,7 @@
       </c>
       <c r="D9" s="1"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B10" s="3" t="s">
         <v>13</v>
       </c>
@@ -909,7 +906,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
         <v>14</v>
       </c>
@@ -917,15 +914,15 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" s="3" t="s">
         <v>15</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.4">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
         <v>16</v>
       </c>
@@ -933,15 +930,15 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B14" s="3" t="s">
         <v>18</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.4">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
         <v>19</v>
       </c>
@@ -949,24 +946,24 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B16" s="3" t="s">
         <v>20</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.4">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B17" s="3" t="s">
         <v>21</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
         <v>23</v>
       </c>
@@ -975,7 +972,7 @@
       </c>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B19" s="3" t="s">
         <v>25</v>
       </c>
@@ -983,7 +980,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B20" s="3" t="s">
         <v>28</v>
       </c>
@@ -991,75 +988,75 @@
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B21" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="D21" s="1"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B22" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C22" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B23" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B24" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B25" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B26" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="D21" s="1"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="B22" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="B23" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="B24" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="B25" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="B26" s="3" t="s">
-        <v>118</v>
-      </c>
       <c r="C26" s="2" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.4">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B27" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="C27" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="C27" s="2" t="s">
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B28" s="3" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="B28" s="3" t="s">
+      <c r="C28" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="C28" s="2" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.4">
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="1"/>
       <c r="B29" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C29" s="11">
         <v>0</v>
@@ -1068,7 +1065,7 @@
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -1076,7 +1073,7 @@
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -1084,179 +1081,179 @@
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="1"/>
       <c r="B32" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A33" s="1"/>
       <c r="B33" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E33" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F33" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="F33" s="1" t="s">
+      <c r="G33" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="G33" s="1" t="s">
+      <c r="H33" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="I33" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="H33" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="I33" s="1" t="s">
-        <v>48</v>
-      </c>
       <c r="J33" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K33" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="L33" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="L33" s="1" t="s">
-        <v>61</v>
-      </c>
       <c r="M33" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="N33" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="N33" s="1" t="s">
+      <c r="O33" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="O33" s="1" t="s">
+      <c r="P33" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="P33" s="1" t="s">
+      <c r="Q33" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="Q33" s="1" t="s">
+      <c r="R33" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="R33" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.4">
+    </row>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A34" s="1"/>
       <c r="B34" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L34" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M34" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N34" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="O34" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="P34" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="Q34" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="R34" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.4">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A35" s="1"/>
       <c r="B35" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J35" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K35" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L35" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="M35" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="N35" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="O35" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="P35" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="Q35" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="R35" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.4">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="36" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -1264,7 +1261,7 @@
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -1272,13 +1269,13 @@
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B44" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C44" s="1"/>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B45" s="1" t="s">
         <v>0</v>
       </c>
@@ -1286,15 +1283,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B46" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.4">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="47" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B47" t="s">
         <v>2</v>
       </c>
@@ -1302,119 +1299,119 @@
         <v>31</v>
       </c>
     </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B48" t="s">
         <v>3</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.4">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B49" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.4">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="50" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B50" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="51" spans="2:3" x14ac:dyDescent="0.4">
-      <c r="B51" t="s">
-        <v>14</v>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="51" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B51" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="52" spans="2:3" x14ac:dyDescent="0.4">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="52" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B52" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C52" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="53" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B53" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C53" s="2" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="53" spans="2:3" x14ac:dyDescent="0.4">
-      <c r="B53" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C53" s="2" t="s">
+    <row r="54" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B54" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C54" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="54" spans="2:3" x14ac:dyDescent="0.4">
-      <c r="B54" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C54" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="55" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="55" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B55" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C55" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="56" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B56" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C56" s="2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="2:3" x14ac:dyDescent="0.4">
-      <c r="B56" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C56" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="57" spans="2:3" x14ac:dyDescent="0.4">
-      <c r="B57" s="1" t="s">
-        <v>21</v>
+    <row r="57" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B57" t="s">
+        <v>56</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="58" spans="2:3" x14ac:dyDescent="0.4">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="58" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B58" t="s">
-        <v>57</v>
+        <v>23</v>
       </c>
       <c r="C58" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="59" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="59" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B59" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="60" spans="2:3" x14ac:dyDescent="0.4">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="60" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B60" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C60" s="2" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="61" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="61" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B61" t="s">
-        <v>28</v>
+        <v>61</v>
       </c>
       <c r="C61" s="2" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="62" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="62" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B62" t="s">
         <v>62</v>
       </c>
@@ -1422,7 +1419,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="63" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="63" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B63" t="s">
         <v>63</v>
       </c>
@@ -1430,20 +1427,12 @@
         <v>69</v>
       </c>
     </row>
-    <row r="64" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="64" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B64" t="s">
         <v>64</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="65" spans="2:3" x14ac:dyDescent="0.4">
-      <c r="B65" t="s">
-        <v>65</v>
-      </c>
-      <c r="C65" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -1459,9 +1448,9 @@
       <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -1469,7 +1458,7 @@
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1477,7 +1466,7 @@
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
         <v>9</v>
@@ -1487,7 +1476,7 @@
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
         <v>0</v>
@@ -1499,7 +1488,7 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
         <v>2</v>
@@ -1511,7 +1500,7 @@
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
       <c r="B6" s="1" t="s">
         <v>3</v>
@@ -1523,7 +1512,7 @@
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
         <v>10</v>
@@ -1535,7 +1524,7 @@
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
       <c r="B8" s="1" t="s">
         <v>13</v>
@@ -1547,7 +1536,7 @@
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>
       <c r="B9" s="1" t="s">
         <v>14</v>
@@ -1559,19 +1548,19 @@
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="1"/>
       <c r="B10" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
         <v>16</v>
       </c>
@@ -1579,15 +1568,15 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.4">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
         <v>19</v>
       </c>
@@ -1595,25 +1584,25 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.4">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="11"/>
       <c r="B15" s="11" t="s">
         <v>21</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D15" s="11"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="11"/>
       <c r="B16" s="11" t="s">
         <v>23</v>
@@ -1623,7 +1612,7 @@
       </c>
       <c r="D16" s="11"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="11"/>
       <c r="B17" s="11" t="s">
         <v>25</v>
@@ -1633,7 +1622,7 @@
       </c>
       <c r="D17" s="11"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="11"/>
       <c r="B18" s="11" t="s">
         <v>28</v>
@@ -1643,93 +1632,93 @@
       </c>
       <c r="D18" s="11"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="11"/>
       <c r="B19" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D19" s="11"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="11"/>
       <c r="B20" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D20" s="11"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="11"/>
       <c r="B21" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D21" s="11"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="11"/>
       <c r="B22" s="11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D22" s="11"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="11"/>
       <c r="B23" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="C23" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="C23" s="11" t="s">
-        <v>78</v>
-      </c>
       <c r="D23" s="11"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="11"/>
       <c r="B24" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="C24" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="C24" s="2" t="s">
-        <v>119</v>
-      </c>
       <c r="D24" s="11"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="11"/>
       <c r="B25" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="C25" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="C25" s="2" t="s">
-        <v>121</v>
-      </c>
       <c r="D25" s="11"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="11"/>
       <c r="B26" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="C26" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="C26" s="2" t="s">
-        <v>123</v>
-      </c>
       <c r="D26" s="11"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="11"/>
       <c r="B27" s="11"/>
       <c r="C27" s="11"/>
       <c r="D27" s="11"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="11"/>
       <c r="B28" s="11"/>
       <c r="C28" s="11"/>
@@ -1744,19 +1733,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0594453C-8787-494B-B55E-35A8780F32ED}">
   <dimension ref="B3:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.4">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B3" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="1"/>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.4">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
@@ -1764,7 +1753,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B5" s="1" t="s">
         <v>2</v>
       </c>
@@ -1772,23 +1761,23 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.4">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B11" s="11" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C11" s="11"/>
       <c r="D11" s="11"/>
       <c r="E11" s="11"/>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.4">
+    <row r="12" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B12" s="11" t="s">
         <v>0</v>
       </c>
@@ -1798,30 +1787,30 @@
       <c r="D12" s="11"/>
       <c r="E12" s="11"/>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.4">
+    <row r="13" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B13" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>127</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>128</v>
       </c>
       <c r="D13" s="11"/>
       <c r="E13" s="11"/>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.4">
+    <row r="14" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B14" s="11"/>
       <c r="C14" s="2"/>
       <c r="D14" s="11"/>
       <c r="E14" s="11"/>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B17" s="11" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C17" s="11"/>
       <c r="D17" s="11"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B18" s="11" t="s">
         <v>0</v>
       </c>
@@ -1830,24 +1819,24 @@
       </c>
       <c r="D18" s="11"/>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.4">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B19" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="C19" s="2" t="s">
-        <v>128</v>
-      </c>
       <c r="D19" s="11"/>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.4">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B21" s="11" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C21" s="11"/>
       <c r="D21" s="11"/>
       <c r="E21" s="11"/>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.4">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B22" s="11" t="s">
         <v>0</v>
       </c>
@@ -1857,12 +1846,12 @@
       <c r="D22" s="11"/>
       <c r="E22" s="11"/>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.4">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B23" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="C23" s="2" t="s">
         <v>127</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>128</v>
       </c>
       <c r="D23" s="11"/>
       <c r="E23" s="11"/>
@@ -1880,15 +1869,15 @@
       <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="2" spans="2:4" s="11" customFormat="1" x14ac:dyDescent="0.4"/>
-    <row r="3" spans="2:4" s="11" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="2:4" s="11" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="3" spans="2:4" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B3" s="11" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="4" spans="2:4" s="11" customFormat="1" x14ac:dyDescent="0.4">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B4" s="11" t="s">
         <v>0</v>
       </c>
@@ -1896,67 +1885,67 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B5" s="11" t="s">
         <v>2</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.4">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B9" s="12"/>
       <c r="D9" s="13"/>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B13" s="11"/>
       <c r="C13" s="10"/>
       <c r="D13" s="9"/>
     </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="16" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B17" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="C17" t="s">
         <v>85</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="D17" s="8" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.4">
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C18" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B19" s="1" t="s">
         <v>83</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="B19" s="1" t="s">
-        <v>84</v>
       </c>
       <c r="C19" s="1">
         <v>1</v>
@@ -1965,9 +1954,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C20" s="1">
         <v>3</v>
@@ -1976,67 +1965,67 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B21" s="6"/>
       <c r="C21" s="5"/>
       <c r="D21" s="4"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="11"/>
       <c r="B22" s="11"/>
       <c r="C22" s="11"/>
       <c r="D22" s="11"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="11"/>
       <c r="B23" s="11" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C23" s="11"/>
       <c r="D23" s="11"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="11"/>
       <c r="B24" s="11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D24" s="11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E24" s="11"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="11"/>
       <c r="B25" s="11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D25" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E25" s="11"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="11"/>
       <c r="B26" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C26" s="11">
         <v>1</v>
       </c>
       <c r="D26" s="11" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.4">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="11"/>
       <c r="B27" s="11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C27" s="11"/>
       <c r="D27" s="11">
@@ -2056,16 +2045,16 @@
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B3" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B4" s="11" t="s">
         <v>0</v>
       </c>
@@ -2074,97 +2063,97 @@
       </c>
       <c r="D4" s="11"/>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B5" s="11" t="s">
         <v>2</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D5" s="11"/>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
       <c r="D6" s="11"/>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B7" s="11"/>
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B9" s="13"/>
       <c r="C9" s="11"/>
       <c r="D9" s="13"/>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B10" s="11"/>
       <c r="C10" s="11"/>
       <c r="D10" s="11"/>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B11" s="11"/>
       <c r="C11" s="11"/>
       <c r="D11" s="11"/>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B12" s="11"/>
       <c r="C12" s="11"/>
       <c r="D12" s="11"/>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B13" s="11"/>
       <c r="C13" s="11"/>
       <c r="D13" s="11"/>
     </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="14" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B14" s="11"/>
       <c r="C14" s="11"/>
       <c r="D14" s="11"/>
     </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="15" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B15" s="11"/>
       <c r="C15" s="11"/>
       <c r="D15" s="11"/>
     </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="16" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B16" s="11" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C16" s="11"/>
       <c r="D16" s="11"/>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B17" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="C17" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="C17" s="11" t="s">
+      <c r="D17" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="D17" s="13" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.4">
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B18" s="11" t="s">
         <v>0</v>
       </c>
       <c r="C18" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="D18" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="D18" s="11" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.4">
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B19" s="11" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C19" s="11">
         <v>1</v>
@@ -2173,9 +2162,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.4">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B20" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C20" s="11">
         <v>3</v>
@@ -2184,54 +2173,54 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.4">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B21" s="11"/>
       <c r="C21" s="11"/>
       <c r="D21" s="11"/>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.4">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B22" s="11"/>
       <c r="C22" s="11"/>
       <c r="D22" s="11"/>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.4">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B23" s="11" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C23" s="11"/>
       <c r="D23" s="11"/>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.4">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B24" s="11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C24" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="D24" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="D24" s="11" t="s">
+      <c r="E24" s="11" t="s">
         <v>106</v>
       </c>
-      <c r="E24" s="11" t="s">
+      <c r="F24" s="11" t="s">
         <v>107</v>
       </c>
-      <c r="F24" s="11" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.4">
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B25" s="11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D25" s="11" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.4">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B26" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C26" s="11"/>
       <c r="D26" s="11"/>
@@ -2239,12 +2228,12 @@
         <v>7</v>
       </c>
       <c r="F26" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.4">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B27" s="11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C27" s="11">
         <v>1</v>

</xml_diff>